<commit_message>
Update invoice template and timesheet formatting
- Removed redundant code sections from the invoice template.
- Updated the timesheet processing logic for better clarity and
  organization.
- Enhanced the flextable formatting for improved presentation of
  timesheet data.
</commit_message>
<xml_diff>
--- a/inst/rmarkdown/templates/invoice/skeleton/resources/timesheet.xlsx
+++ b/inst/rmarkdown/templates/invoice/skeleton/resources/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marai\Workspace\Packages\wihantemplates\inst\rmarkdown\templates\invoice\skeleton\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F0191F-6BDF-45EF-BA63-3A7CE4A9D330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3212B735-5A0A-4458-9B88-00D509A0372C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,58 +50,58 @@
     <t>Z</t>
   </si>
   <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>Design new carousel</t>
-  </si>
-  <si>
-    <t>Coordinate lighting installation</t>
-  </si>
-  <si>
-    <t>Review attraction blueprints</t>
-  </si>
-  <si>
-    <t>Install safety barriers</t>
-  </si>
-  <si>
-    <t>Test ride systems</t>
-  </si>
-  <si>
-    <t>Train staff on new attractions</t>
-  </si>
-  <si>
-    <t>Conduct safety inspections</t>
-  </si>
-  <si>
-    <t>Update project management software</t>
-  </si>
-  <si>
-    <t>Coordinate with vendors</t>
-  </si>
-  <si>
-    <t>Finalize attraction signage</t>
-  </si>
-  <si>
-    <t>Prepare presentation for stakeholders</t>
-  </si>
-  <si>
-    <t>Update budget forecasts</t>
-  </si>
-  <si>
-    <t>Manage supply chain logistics</t>
-  </si>
-  <si>
-    <t>Conduct staff training sessions</t>
-  </si>
-  <si>
-    <t>Final quality assurance checks</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial concept sketches for new attraction area </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site layout planning and space allocation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental impact assessment of new structures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Character meet-and-greet zone design </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic flow analysis for expanded visitor capacity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facade detailing for themed restaurant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water feature integration planning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lighting design for nighttime operations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visitor experience impact study for construction period </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundation assessment for main attraction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guest flow optimization for new pathways </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theming coordination with creative team </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility compliance review </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety protocol documentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final design review with client </t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,16 +483,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -500,7 +500,7 @@
         <v>45292</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5">
         <v>0.33333333333333331</v>
@@ -514,10 +514,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>45293</v>
+        <v>45292</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5">
         <v>0.38541666666666669</v>
@@ -534,7 +534,7 @@
         <v>45294</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
         <v>0.3125</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>45295</v>
+        <v>45294</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5">
         <v>0.41666666666666669</v>
@@ -568,7 +568,7 @@
         <v>45296</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5">
         <v>0.54166666666666663</v>
@@ -585,7 +585,7 @@
         <v>45297</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5">
         <v>0.625</v>
@@ -602,7 +602,7 @@
         <v>45298</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5">
         <v>0.35416666666666669</v>
@@ -619,7 +619,7 @@
         <v>45299</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5">
         <v>0.44791666666666669</v>
@@ -633,10 +633,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>45300</v>
+        <v>45299</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5">
         <v>0.58333333333333337</v>
@@ -653,7 +653,7 @@
         <v>45301</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5">
         <v>0.375</v>
@@ -670,7 +670,7 @@
         <v>45302</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5">
         <v>0.32291666666666669</v>
@@ -684,10 +684,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>45303</v>
+        <v>45302</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5">
         <v>0.4375</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>45304</v>
+        <v>45302</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5">
         <v>0.5</v>
@@ -721,7 +721,7 @@
         <v>45305</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5">
         <v>0.59375</v>
@@ -738,7 +738,7 @@
         <v>45306</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5">
         <v>0.66666666666666663</v>
@@ -752,5 +752,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>